<commit_message>
Mise à jour income_statementDB
</commit_message>
<xml_diff>
--- a/0.0.Template/income_statement_DB_file.xlsx
+++ b/0.0.Template/income_statement_DB_file.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AK1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,187 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Hello world !</t>
+          <t>Nature comptable</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Designation comptable</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Centre de coût</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Designation centre de coût</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Centre de profit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Designation centre de profit</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Montant</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Type Piece</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Nom</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Prenom</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Matricule</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Periode d'effet</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Debut periode</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Fin periode</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>N° piece reference</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Utilisateur ecriture</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Date piece</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Date comptable</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Date de saisie</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Compte contre partie</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Designation compte contre partie</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>N° Ecriture</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Commentaire ecriture</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>N° contre passation</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Commentaire contre passation</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Devise</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Convertion en euros</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>Date convertion</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>Taux convertion</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>Source convertion</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>Societe</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>Designation societe</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>Unité de quantité</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>Quantité</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>Taux unité de quantité</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>Code mouvement</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>Designation mouvement</t>
         </is>
       </c>
     </row>

</xml_diff>